<commit_message>
Added remap for Nilou --> NilouBreeze
- colour of NilouBreeze's outline need to be fixed
(probably need to find the correct hash to apply the shader fix starter
adhoc code)
</commit_message>
<xml_diff>
--- a/Data/RemapDrafts/ShenheRemapDraft.xlsx
+++ b/Data/RemapDrafts/ShenheRemapDraft.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer\Games\Genshin\Repos\Repos\Fix-Raiden-Boss-Fork\Data\RemapDrafts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer\Games\Genshin\Repos\Repos\Fix-Raiden-Boss\Data\RemapDrafts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78423494-C2C4-47A1-8DA7-323E26C5B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799BB872-8BFC-45B5-B45F-4C4AE77FFC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15720" xr2:uid="{3D0650C5-DBE0-4C90-9415-3AA816221020}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15720" activeTab="1" xr2:uid="{3D0650C5-DBE0-4C90-9415-3AA816221020}"/>
   </bookViews>
   <sheets>
-    <sheet name="Shenhe to ShenheFrostFlower" sheetId="1" r:id="rId1"/>
-    <sheet name="SheheFrostFlower to Shenhe" sheetId="2" r:id="rId2"/>
+    <sheet name="V4.4Shenhe to ShenheFrostFlower" sheetId="1" r:id="rId1"/>
+    <sheet name="V4.4SheheFrostFlower to Shenhe" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Shenhe to ShenheFrostFlower'!$A$1:$D$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V4.4Shenhe to ShenheFrostFlower'!$A$1:$D$111</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2583E74-8F82-4F81-B04F-19E52E22920E}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1679,7 +1679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979D0712-8E47-4847-ADBC-0D4AB264156A}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>